<commit_message>
Wrangling for network visualization
</commit_message>
<xml_diff>
--- a/data/CrudeOilExports.xlsx
+++ b/data/CrudeOilExports.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\USERS\DSSEP1\SEC\Annual Statistical Bulletin (ASB)\ASB 2023\2 Tables Electronic Version\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanvandewater/Data-Science/vandewater-ethan/Internet_Explorers/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED9EEBC-03AD-7C45-873B-75F1E3DBCC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="450" windowWidth="23760" windowHeight="10200"/>
+    <workbookView xWindow="1380" yWindow="500" windowWidth="25960" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 5.2" sheetId="1" r:id="rId1"/>
@@ -23,9 +24,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
-  <si>
-    <t xml:space="preserve">                    </t>
-  </si>
   <si>
     <t>OPEC</t>
   </si>
@@ -254,18 +252,21 @@
   <si>
     <t>© 2023 Organization of the Petroleum Exporting Countries</t>
   </si>
+  <si>
+    <t>Country</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="yyyy"/>
     <numFmt numFmtId="167" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -420,6 +421,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -487,82 +496,82 @@
   </cellStyleXfs>
   <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="4" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="4" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="19" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="19" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="2" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="2" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="2" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="2" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="19" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -571,49 +580,51 @@
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="2" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="22" fillId="2" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="24" fillId="4" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="27">
-    <cellStyle name="Comma 2" xfId="1"/>
+    <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="2"/>
-    <cellStyle name="Normal 103" xfId="3"/>
-    <cellStyle name="Normal 2" xfId="4"/>
-    <cellStyle name="Normal 2 10" xfId="5"/>
-    <cellStyle name="Normal 2 2" xfId="6"/>
-    <cellStyle name="Normal 2 2 2" xfId="7"/>
-    <cellStyle name="Normal 2 2 3" xfId="8"/>
-    <cellStyle name="Normal 21" xfId="9"/>
-    <cellStyle name="Normal 3" xfId="10"/>
-    <cellStyle name="Normal 3 11" xfId="11"/>
-    <cellStyle name="Normal 3 2" xfId="12"/>
-    <cellStyle name="Normal 3 3" xfId="13"/>
-    <cellStyle name="Normal 4" xfId="14"/>
-    <cellStyle name="Normal 4 2 3" xfId="15"/>
-    <cellStyle name="Normal 5" xfId="16"/>
-    <cellStyle name="Normal_Sheet1_1" xfId="17"/>
-    <cellStyle name="Normal_Sheet1_2" xfId="18"/>
-    <cellStyle name="Normal_T52p" xfId="19"/>
+    <cellStyle name="Normal 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 103" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2 10" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2 2 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 2 2 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 21" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 3" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 3 11" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 3 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 4" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 4 2 3" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 5" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal_Sheet1_1" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal_Sheet1_2" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal_T52p" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
     <cellStyle name="Percent" xfId="20" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="21"/>
-    <cellStyle name="Percent 2 2" xfId="22"/>
-    <cellStyle name="Percent 2 3" xfId="23"/>
-    <cellStyle name="Percent 3" xfId="24"/>
-    <cellStyle name="Percent 4" xfId="25"/>
-    <cellStyle name="Vírgula 2" xfId="26"/>
+    <cellStyle name="Percent 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Percent 2 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Percent 2 3" xfId="23" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Percent 3" xfId="24" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Percent 4" xfId="25" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Vírgula 2" xfId="26" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -718,9 +729,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -758,9 +769,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -795,7 +806,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -830,7 +841,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1003,28 +1014,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AR93"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="O29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3:AR3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="44" width="7.85546875" style="1" customWidth="1"/>
-    <col min="45" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="31.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="44" width="7.83203125" style="1" customWidth="1"/>
+    <col min="45" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" ht="17">
       <c r="A1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -1070,9 +1081,9 @@
       <c r="AQ1" s="31"/>
       <c r="AR1" s="31"/>
     </row>
-    <row r="2" spans="1:44" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:44" ht="34">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1118,143 +1129,143 @@
       <c r="AQ2" s="26"/>
       <c r="AR2" s="26"/>
     </row>
-    <row r="3" spans="1:44" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="6">
-        <v>29221</v>
-      </c>
-      <c r="C3" s="6">
-        <v>29587</v>
-      </c>
-      <c r="D3" s="6">
-        <v>29952</v>
-      </c>
-      <c r="E3" s="6">
-        <v>30317</v>
-      </c>
-      <c r="F3" s="6">
-        <v>30682</v>
-      </c>
-      <c r="G3" s="6">
-        <v>31048</v>
-      </c>
-      <c r="H3" s="6">
-        <v>31413</v>
-      </c>
-      <c r="I3" s="6">
-        <v>31778</v>
-      </c>
-      <c r="J3" s="6">
-        <v>32143</v>
-      </c>
-      <c r="K3" s="6">
-        <v>32509</v>
-      </c>
-      <c r="L3" s="6">
-        <v>32874</v>
-      </c>
-      <c r="M3" s="6">
-        <v>33239</v>
-      </c>
-      <c r="N3" s="6">
-        <v>33604</v>
-      </c>
-      <c r="O3" s="6">
-        <v>33970</v>
-      </c>
-      <c r="P3" s="6">
-        <v>34335</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>34700</v>
-      </c>
-      <c r="R3" s="6">
-        <v>35065</v>
-      </c>
-      <c r="S3" s="6">
-        <v>35431</v>
-      </c>
-      <c r="T3" s="6">
-        <v>35796</v>
-      </c>
-      <c r="U3" s="6">
-        <v>36161</v>
-      </c>
-      <c r="V3" s="6">
-        <v>36526</v>
-      </c>
-      <c r="W3" s="6">
-        <v>36892</v>
-      </c>
-      <c r="X3" s="6">
-        <v>37257</v>
-      </c>
-      <c r="Y3" s="6">
-        <v>37622</v>
-      </c>
-      <c r="Z3" s="6">
-        <v>37987</v>
-      </c>
-      <c r="AA3" s="6">
-        <v>38353</v>
-      </c>
-      <c r="AB3" s="6">
-        <v>38718</v>
-      </c>
-      <c r="AC3" s="6">
-        <v>39083</v>
-      </c>
-      <c r="AD3" s="6">
-        <v>39448</v>
-      </c>
-      <c r="AE3" s="6">
-        <v>39814</v>
-      </c>
-      <c r="AF3" s="6">
-        <v>40179</v>
-      </c>
-      <c r="AG3" s="6">
-        <v>40544</v>
-      </c>
-      <c r="AH3" s="6">
-        <v>40909</v>
-      </c>
-      <c r="AI3" s="6">
-        <v>41275</v>
-      </c>
-      <c r="AJ3" s="6">
-        <v>41640</v>
-      </c>
-      <c r="AK3" s="6">
-        <v>42005</v>
-      </c>
-      <c r="AL3" s="6">
-        <v>42370</v>
-      </c>
-      <c r="AM3" s="6">
-        <v>42736</v>
-      </c>
-      <c r="AN3" s="6">
-        <v>43101</v>
-      </c>
-      <c r="AO3" s="6">
-        <v>43466</v>
-      </c>
-      <c r="AP3" s="6">
-        <v>43831</v>
-      </c>
-      <c r="AQ3" s="6">
-        <v>44197</v>
-      </c>
-      <c r="AR3" s="6">
-        <v>44562</v>
+        <v>58</v>
+      </c>
+      <c r="B3" s="40">
+        <v>1980</v>
+      </c>
+      <c r="C3" s="40">
+        <v>1981</v>
+      </c>
+      <c r="D3" s="40">
+        <v>1982</v>
+      </c>
+      <c r="E3" s="40">
+        <v>1983</v>
+      </c>
+      <c r="F3" s="40">
+        <v>1984</v>
+      </c>
+      <c r="G3" s="40">
+        <v>1985</v>
+      </c>
+      <c r="H3" s="40">
+        <v>1986</v>
+      </c>
+      <c r="I3" s="40">
+        <v>1987</v>
+      </c>
+      <c r="J3" s="40">
+        <v>1988</v>
+      </c>
+      <c r="K3" s="40">
+        <v>1989</v>
+      </c>
+      <c r="L3" s="40">
+        <v>1990</v>
+      </c>
+      <c r="M3" s="40">
+        <v>1991</v>
+      </c>
+      <c r="N3" s="40">
+        <v>1992</v>
+      </c>
+      <c r="O3" s="40">
+        <v>1993</v>
+      </c>
+      <c r="P3" s="40">
+        <v>1994</v>
+      </c>
+      <c r="Q3" s="40">
+        <v>1995</v>
+      </c>
+      <c r="R3" s="40">
+        <v>1996</v>
+      </c>
+      <c r="S3" s="40">
+        <v>1997</v>
+      </c>
+      <c r="T3" s="40">
+        <v>1998</v>
+      </c>
+      <c r="U3" s="40">
+        <v>1999</v>
+      </c>
+      <c r="V3" s="40">
+        <v>2000</v>
+      </c>
+      <c r="W3" s="40">
+        <v>2001</v>
+      </c>
+      <c r="X3" s="40">
+        <v>2002</v>
+      </c>
+      <c r="Y3" s="40">
+        <v>2003</v>
+      </c>
+      <c r="Z3" s="40">
+        <v>2004</v>
+      </c>
+      <c r="AA3" s="40">
+        <v>2005</v>
+      </c>
+      <c r="AB3" s="40">
+        <v>2006</v>
+      </c>
+      <c r="AC3" s="40">
+        <v>2007</v>
+      </c>
+      <c r="AD3" s="40">
+        <v>2008</v>
+      </c>
+      <c r="AE3" s="40">
+        <v>2009</v>
+      </c>
+      <c r="AF3" s="40">
+        <v>2010</v>
+      </c>
+      <c r="AG3" s="40">
+        <v>2011</v>
+      </c>
+      <c r="AH3" s="40">
+        <v>2012</v>
+      </c>
+      <c r="AI3" s="40">
+        <v>2013</v>
+      </c>
+      <c r="AJ3" s="40">
+        <v>2014</v>
+      </c>
+      <c r="AK3" s="40">
+        <v>2015</v>
+      </c>
+      <c r="AL3" s="40">
+        <v>2016</v>
+      </c>
+      <c r="AM3" s="40">
+        <v>2017</v>
+      </c>
+      <c r="AN3" s="40">
+        <v>2018</v>
+      </c>
+      <c r="AO3" s="40">
+        <v>2019</v>
+      </c>
+      <c r="AP3" s="40">
+        <v>2020</v>
+      </c>
+      <c r="AQ3" s="40">
+        <v>2021</v>
+      </c>
+      <c r="AR3" s="40">
+        <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:44" ht="15" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="20">
         <v>1412.8677260273971</v>
@@ -1386,9 +1397,9 @@
         <v>7967.1813424657539</v>
       </c>
     </row>
-    <row r="5" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" ht="15" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="21">
         <v>205.06772602739727</v>
@@ -1520,9 +1531,9 @@
         <v>3350.2000821917809</v>
       </c>
     </row>
-    <row r="6" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" ht="15" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="21">
         <v>920.8</v>
@@ -1654,9 +1665,9 @@
         <v>1011.7899452054795</v>
       </c>
     </row>
-    <row r="7" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" ht="15" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="21">
         <v>287</v>
@@ -1788,9 +1799,9 @@
         <v>3604</v>
       </c>
     </row>
-    <row r="8" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44" ht="15" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="21">
         <v>0</v>
@@ -1922,9 +1933,9 @@
         <v>1.1913150684931506</v>
       </c>
     </row>
-    <row r="9" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:44" ht="15" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="20">
         <v>1467.1938251366123</v>
@@ -2056,9 +2067,9 @@
         <v>2130.9193972602739</v>
       </c>
     </row>
-    <row r="10" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44" ht="15" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="21">
         <v>401.81643835616438</v>
@@ -2190,9 +2201,9 @@
         <v>1558.1593424657535</v>
       </c>
     </row>
-    <row r="11" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:44" ht="15" customHeight="1">
       <c r="A11" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="21">
         <v>785.4</v>
@@ -2324,9 +2335,9 @@
         <v>540.19071232876718</v>
       </c>
     </row>
-    <row r="12" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:44" ht="15" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="21">
         <v>279.97738678044777</v>
@@ -2458,9 +2469,9 @@
         <v>32.56934246575338</v>
       </c>
     </row>
-    <row r="13" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:44" ht="15" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="20">
         <v>0</v>
@@ -2592,9 +2603,9 @@
         <v>257.14232876712327</v>
       </c>
     </row>
-    <row r="14" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:44" ht="15" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="21">
         <v>0</v>
@@ -2726,9 +2737,9 @@
         <v>243.5734520547945</v>
       </c>
     </row>
-    <row r="15" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:44" ht="15" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="21">
         <v>0</v>
@@ -2860,9 +2871,9 @@
         <v>13.568876712328773</v>
       </c>
     </row>
-    <row r="16" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:44" ht="15" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="20">
         <v>266.90926000000002</v>
@@ -2994,9 +3005,9 @@
         <v>41.489317258251923</v>
       </c>
     </row>
-    <row r="17" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:44" ht="15" customHeight="1">
       <c r="A17" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="20">
         <v>0</v>
@@ -3128,9 +3139,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:44" ht="15" customHeight="1">
       <c r="A18" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="20">
         <v>1677.4147953700001</v>
@@ -3262,9 +3273,9 @@
         <v>414.31949649673822</v>
       </c>
     </row>
-    <row r="19" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:44" ht="15" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="21">
         <v>219.25484900000001</v>
@@ -3396,9 +3407,9 @@
         <v>38.916666666666664</v>
       </c>
     </row>
-    <row r="20" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:44" ht="15" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="21">
         <v>1211.3624400000001</v>
@@ -3530,9 +3541,9 @@
         <v>39.583333333333336</v>
       </c>
     </row>
-    <row r="21" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:44" ht="15" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="21">
         <v>239.99120500000001</v>
@@ -3664,9 +3675,9 @@
         <v>203.33333333333334</v>
       </c>
     </row>
-    <row r="22" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:44" ht="15" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="21">
         <v>0</v>
@@ -3798,9 +3809,9 @@
         <v>55.083333333333336</v>
       </c>
     </row>
-    <row r="23" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:44" ht="15" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="21">
         <v>6.8063013699999999</v>
@@ -3932,9 +3943,9 @@
         <v>77.402829830071553</v>
       </c>
     </row>
-    <row r="24" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:44" ht="15" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="20">
         <v>1598.7324931312328</v>
@@ -4066,9 +4077,9 @@
         <v>3059.9399771689505</v>
       </c>
     </row>
-    <row r="25" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:44" ht="15" customHeight="1">
       <c r="A25" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="22">
         <v>1.2032876712328768</v>
@@ -4200,9 +4211,9 @@
         <v>1346.4166666666667</v>
       </c>
     </row>
-    <row r="26" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:44" ht="15" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="21">
         <v>0</v>
@@ -4334,9 +4345,9 @@
         <v>487</v>
       </c>
     </row>
-    <row r="27" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:44" ht="15" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B27" s="21">
         <v>112.9</v>
@@ -4468,9 +4479,9 @@
         <v>313.33333333333331</v>
       </c>
     </row>
-    <row r="28" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:44" ht="15" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="21">
         <v>126.9</v>
@@ -4602,9 +4613,9 @@
         <v>54.083333333333336</v>
       </c>
     </row>
-    <row r="29" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:44" ht="15" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" s="21">
         <v>1287.2</v>
@@ -4736,9 +4747,9 @@
         <v>438.17341095890487</v>
       </c>
     </row>
-    <row r="30" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:44" ht="15" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" s="21">
         <v>70.52920546</v>
@@ -4870,9 +4881,9 @@
         <v>420.93323287671251</v>
       </c>
     </row>
-    <row r="31" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:44" ht="15" customHeight="1">
       <c r="A31" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" s="20">
         <v>16375.8</v>
@@ -5004,9 +5015,9 @@
         <v>18154.983005660641</v>
       </c>
     </row>
-    <row r="32" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:44" ht="15" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" s="21">
         <v>0</v>
@@ -5138,9 +5149,9 @@
         <v>151.58333333333334</v>
       </c>
     </row>
-    <row r="33" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:44" ht="15" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="21">
         <v>796.7</v>
@@ -5272,9 +5283,9 @@
         <v>900.63183333333336</v>
       </c>
     </row>
-    <row r="34" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:44" ht="15" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B34" s="21">
         <v>2482</v>
@@ -5406,9 +5417,9 @@
         <v>3712.42</v>
       </c>
     </row>
-    <row r="35" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:44" ht="15" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B35" s="21">
         <v>1296.5</v>
@@ -5540,9 +5551,9 @@
         <v>1878.8515833333333</v>
       </c>
     </row>
-    <row r="36" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:44" ht="15" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B36" s="21">
         <v>286.89999999999998</v>
@@ -5674,9 +5685,9 @@
         <v>921.80308333333323</v>
       </c>
     </row>
-    <row r="37" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:44" ht="15" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B37" s="21">
         <v>465.7</v>
@@ -5808,9 +5819,9 @@
         <v>475.35313899397607</v>
       </c>
     </row>
-    <row r="38" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:44" ht="15" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B38" s="21">
         <v>9223.2000000000007</v>
@@ -5942,9 +5953,9 @@
         <v>7363.64</v>
       </c>
     </row>
-    <row r="39" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:44" ht="15" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B39" s="21">
         <v>1697.3</v>
@@ -6076,9 +6087,9 @@
         <v>2717.1167000000005</v>
       </c>
     </row>
-    <row r="40" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:44" ht="15" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40" s="21">
         <v>127.5</v>
@@ -6210,9 +6221,9 @@
         <v>33.583333333333336</v>
       </c>
     </row>
-    <row r="41" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:44" ht="15" customHeight="1">
       <c r="A41" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41" s="20">
         <v>5428.9815884999989</v>
@@ -6344,9 +6355,9 @@
         <v>4841.020605138905</v>
       </c>
     </row>
-    <row r="42" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:44" ht="15" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42" s="21">
         <v>715.5</v>
@@ -6478,9 +6489,9 @@
         <v>476.89617260273974</v>
       </c>
     </row>
-    <row r="43" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:44" ht="15" customHeight="1">
       <c r="A43" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B43" s="21">
         <v>332.8</v>
@@ -6612,9 +6623,9 @@
         <v>1084.9105029041095</v>
       </c>
     </row>
-    <row r="44" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:44" ht="15" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B44" s="21">
         <v>65.125479499999997</v>
@@ -6746,9 +6757,9 @@
         <v>242.83875000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:44" ht="15" customHeight="1">
       <c r="A45" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B45" s="21">
         <v>335.67057499999999</v>
@@ -6880,9 +6891,9 @@
         <v>71.083333333333329</v>
       </c>
     </row>
-    <row r="46" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:44" ht="15" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="21">
         <v>0</v>
@@ -7014,9 +7025,9 @@
         <v>80.721277348950338</v>
       </c>
     </row>
-    <row r="47" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:44" ht="15" customHeight="1">
       <c r="A47" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B47" s="21">
         <v>150.24553399999999</v>
@@ -7148,9 +7159,9 @@
         <v>184.91049999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:44" ht="15" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B48" s="21">
         <v>1693</v>
@@ -7282,9 +7293,9 @@
         <v>919.82799999999997</v>
       </c>
     </row>
-    <row r="49" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:44" ht="15" customHeight="1">
       <c r="A49" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B49" s="21">
         <v>1960.2</v>
@@ -7416,9 +7427,9 @@
         <v>1388.2602356164382</v>
       </c>
     </row>
-    <row r="50" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:44" ht="15" customHeight="1">
       <c r="A50" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B50" s="21">
         <v>0</v>
@@ -7550,9 +7561,9 @@
         <v>116.40516666666667</v>
       </c>
     </row>
-    <row r="51" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:44" ht="15" customHeight="1">
       <c r="A51" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B51" s="21">
         <v>176.44</v>
@@ -7684,9 +7695,9 @@
         <v>275.16666666666669</v>
       </c>
     </row>
-    <row r="52" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:44" ht="15" customHeight="1">
       <c r="A52" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B52" s="20">
         <v>4530.850614</v>
@@ -7818,9 +7829,9 @@
         <v>4780.3543333333337</v>
       </c>
     </row>
-    <row r="53" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:44" ht="15" customHeight="1">
       <c r="A53" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B53" s="20">
         <v>0.58820974623850475</v>
@@ -7952,39 +7963,39 @@
         <v>1812.5486034782609</v>
       </c>
     </row>
-    <row r="54" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:44" ht="15" customHeight="1">
       <c r="A54" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G54" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H54" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I54" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J54" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K54" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L54" s="21">
         <v>0</v>
@@ -8086,39 +8097,39 @@
         <v>441.33333333333331</v>
       </c>
     </row>
-    <row r="55" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:44" ht="15" customHeight="1">
       <c r="A55" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G55" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H55" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I55" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J55" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K55" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L55" s="21">
         <v>405.92909589041096</v>
@@ -8220,9 +8231,9 @@
         <v>1315.1666666666667</v>
       </c>
     </row>
-    <row r="56" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:44" ht="15" customHeight="1">
       <c r="A56" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B56" s="21">
         <v>0.58820974623850475</v>
@@ -8354,9 +8365,9 @@
         <v>56.048603478260851</v>
       </c>
     </row>
-    <row r="57" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:44" ht="15" customHeight="1">
       <c r="A57" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B57" s="20">
         <v>0</v>
@@ -8488,9 +8499,9 @@
         <v>17.416666666666668</v>
       </c>
     </row>
-    <row r="58" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:44" ht="15" customHeight="1">
       <c r="A58" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B58" s="20">
         <v>32759.338511911479</v>
@@ -8622,9 +8633,9 @@
         <v>43477.315073694896</v>
       </c>
     </row>
-    <row r="59" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:44" ht="15" customHeight="1">
       <c r="A59" s="10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B59" s="23"/>
       <c r="C59" s="23"/>
@@ -8653,26 +8664,26 @@
       <c r="Z59" s="23"/>
       <c r="AA59" s="23"/>
       <c r="AB59" s="24"/>
-      <c r="AC59" s="37"/>
-      <c r="AD59" s="37"/>
-      <c r="AE59" s="37"/>
-      <c r="AF59" s="37"/>
-      <c r="AG59" s="37"/>
-      <c r="AH59" s="37"/>
-      <c r="AI59" s="37"/>
-      <c r="AJ59" s="37"/>
-      <c r="AK59" s="37"/>
-      <c r="AL59" s="37"/>
-      <c r="AM59" s="37"/>
-      <c r="AN59" s="37"/>
-      <c r="AO59" s="37"/>
-      <c r="AP59" s="37"/>
-      <c r="AQ59" s="37"/>
-      <c r="AR59" s="37"/>
+      <c r="AC59" s="36"/>
+      <c r="AD59" s="36"/>
+      <c r="AE59" s="36"/>
+      <c r="AF59" s="36"/>
+      <c r="AG59" s="36"/>
+      <c r="AH59" s="36"/>
+      <c r="AI59" s="36"/>
+      <c r="AJ59" s="36"/>
+      <c r="AK59" s="36"/>
+      <c r="AL59" s="36"/>
+      <c r="AM59" s="36"/>
+      <c r="AN59" s="36"/>
+      <c r="AO59" s="36"/>
+      <c r="AP59" s="36"/>
+      <c r="AQ59" s="36"/>
+      <c r="AR59" s="36"/>
     </row>
-    <row r="60" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:44" ht="15" customHeight="1">
       <c r="A60" s="11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B60" s="23">
         <v>21699.771013500002</v>
@@ -8804,9 +8815,9 @@
         <v>21389.198966097818</v>
       </c>
     </row>
-    <row r="61" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:44" ht="15" customHeight="1">
       <c r="A61" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B61" s="13">
         <v>66.239954770789538</v>
@@ -8938,9 +8949,9 @@
         <v>49.196227802574079</v>
       </c>
     </row>
-    <row r="62" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:44" ht="14">
       <c r="A62" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B62" s="23">
         <v>2880.0615511640094</v>
@@ -9072,7 +9083,7 @@
         <v>10355.243068493151</v>
       </c>
     </row>
-    <row r="63" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:44">
       <c r="A63" s="14"/>
       <c r="B63" s="15"/>
       <c r="C63" s="16"/>
@@ -9099,15 +9110,15 @@
       <c r="X63" s="16"/>
       <c r="Y63" s="16"/>
       <c r="Z63" s="16"/>
-      <c r="AA63" s="38"/>
-      <c r="AB63" s="38"/>
-      <c r="AC63" s="38"/>
-      <c r="AD63" s="38"/>
-      <c r="AE63" s="38"/>
-      <c r="AF63" s="38"/>
-      <c r="AG63" s="38"/>
-      <c r="AH63" s="38"/>
-      <c r="AI63" s="38"/>
+      <c r="AA63" s="37"/>
+      <c r="AB63" s="37"/>
+      <c r="AC63" s="37"/>
+      <c r="AD63" s="37"/>
+      <c r="AE63" s="37"/>
+      <c r="AF63" s="37"/>
+      <c r="AG63" s="37"/>
+      <c r="AH63" s="37"/>
+      <c r="AI63" s="37"/>
       <c r="AJ63" s="35"/>
       <c r="AK63" s="35"/>
       <c r="AL63" s="35"/>
@@ -9118,9 +9129,9 @@
       <c r="AQ63" s="35"/>
       <c r="AR63" s="35"/>
     </row>
-    <row r="64" spans="1:44" s="3" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:44" s="3" customFormat="1" ht="30">
       <c r="A64" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B64" s="17"/>
       <c r="C64" s="18"/>
@@ -9166,53 +9177,53 @@
       <c r="AQ64" s="18"/>
       <c r="AR64" s="18"/>
     </row>
-    <row r="65" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:44" s="3" customFormat="1" ht="14">
       <c r="A65" s="32"/>
-      <c r="B65" s="39"/>
-      <c r="C65" s="39"/>
-      <c r="D65" s="39"/>
-      <c r="E65" s="39"/>
-      <c r="F65" s="39"/>
-      <c r="G65" s="39"/>
-      <c r="H65" s="39"/>
-      <c r="I65" s="39"/>
-      <c r="J65" s="39"/>
-      <c r="K65" s="39"/>
-      <c r="L65" s="39"/>
-      <c r="M65" s="39"/>
-      <c r="N65" s="39"/>
-      <c r="O65" s="39"/>
-      <c r="P65" s="39"/>
-      <c r="Q65" s="39"/>
-      <c r="R65" s="39"/>
-      <c r="S65" s="39"/>
-      <c r="T65" s="39"/>
-      <c r="U65" s="39"/>
-      <c r="V65" s="39"/>
-      <c r="W65" s="39"/>
-      <c r="X65" s="39"/>
-      <c r="Y65" s="39"/>
-      <c r="Z65" s="39"/>
-      <c r="AA65" s="39"/>
-      <c r="AB65" s="39"/>
-      <c r="AC65" s="39"/>
-      <c r="AD65" s="39"/>
-      <c r="AE65" s="39"/>
-      <c r="AF65" s="39"/>
-      <c r="AG65" s="39"/>
-      <c r="AH65" s="39"/>
-      <c r="AI65" s="39"/>
-      <c r="AJ65" s="39"/>
-      <c r="AK65" s="39"/>
-      <c r="AL65" s="39"/>
-      <c r="AM65" s="39"/>
-      <c r="AN65" s="39"/>
-      <c r="AO65" s="39"/>
-      <c r="AP65" s="39"/>
-      <c r="AQ65" s="39"/>
-      <c r="AR65" s="39"/>
+      <c r="B65" s="38"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="38"/>
+      <c r="G65" s="38"/>
+      <c r="H65" s="38"/>
+      <c r="I65" s="38"/>
+      <c r="J65" s="38"/>
+      <c r="K65" s="38"/>
+      <c r="L65" s="38"/>
+      <c r="M65" s="38"/>
+      <c r="N65" s="38"/>
+      <c r="O65" s="38"/>
+      <c r="P65" s="38"/>
+      <c r="Q65" s="38"/>
+      <c r="R65" s="38"/>
+      <c r="S65" s="38"/>
+      <c r="T65" s="38"/>
+      <c r="U65" s="38"/>
+      <c r="V65" s="38"/>
+      <c r="W65" s="38"/>
+      <c r="X65" s="38"/>
+      <c r="Y65" s="38"/>
+      <c r="Z65" s="38"/>
+      <c r="AA65" s="38"/>
+      <c r="AB65" s="38"/>
+      <c r="AC65" s="38"/>
+      <c r="AD65" s="38"/>
+      <c r="AE65" s="38"/>
+      <c r="AF65" s="38"/>
+      <c r="AG65" s="38"/>
+      <c r="AH65" s="38"/>
+      <c r="AI65" s="38"/>
+      <c r="AJ65" s="38"/>
+      <c r="AK65" s="38"/>
+      <c r="AL65" s="38"/>
+      <c r="AM65" s="38"/>
+      <c r="AN65" s="38"/>
+      <c r="AO65" s="38"/>
+      <c r="AP65" s="38"/>
+      <c r="AQ65" s="38"/>
+      <c r="AR65" s="38"/>
     </row>
-    <row r="66" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:44" s="3" customFormat="1">
       <c r="A66" s="1"/>
       <c r="B66" s="30"/>
       <c r="C66" s="30"/>
@@ -9258,9 +9269,9 @@
       <c r="AQ66" s="30"/>
       <c r="AR66" s="30"/>
     </row>
-    <row r="67" spans="1:44" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:44" s="33" customFormat="1" ht="14">
       <c r="A67" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B67" s="28"/>
       <c r="C67" s="28"/>
@@ -9270,43 +9281,8 @@
       <c r="G67" s="28"/>
       <c r="H67" s="28"/>
       <c r="I67" s="28"/>
-      <c r="J67" s="33"/>
-      <c r="K67" s="33"/>
-      <c r="L67" s="33"/>
-      <c r="M67" s="33"/>
-      <c r="N67" s="33"/>
-      <c r="O67" s="33"/>
-      <c r="P67" s="33"/>
-      <c r="Q67" s="33"/>
-      <c r="R67" s="33"/>
-      <c r="S67" s="33"/>
-      <c r="T67" s="33"/>
-      <c r="U67" s="33"/>
-      <c r="V67" s="33"/>
-      <c r="W67" s="33"/>
-      <c r="X67" s="33"/>
-      <c r="Y67" s="33"/>
-      <c r="Z67" s="33"/>
-      <c r="AA67" s="33"/>
-      <c r="AB67" s="33"/>
-      <c r="AC67" s="33"/>
-      <c r="AD67" s="33"/>
-      <c r="AE67" s="33"/>
-      <c r="AF67" s="33"/>
-      <c r="AG67" s="33"/>
-      <c r="AH67" s="33"/>
-      <c r="AI67" s="33"/>
-      <c r="AJ67" s="33"/>
-      <c r="AK67" s="33"/>
-      <c r="AL67" s="33"/>
-      <c r="AM67" s="33"/>
-      <c r="AN67" s="33"/>
-      <c r="AO67" s="33"/>
-      <c r="AP67" s="33"/>
-      <c r="AQ67" s="33"/>
-      <c r="AR67" s="33"/>
     </row>
-    <row r="68" spans="1:44" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:44" s="33" customFormat="1" ht="14">
       <c r="A68" s="29"/>
       <c r="B68" s="28"/>
       <c r="C68" s="28"/>
@@ -9316,43 +9292,8 @@
       <c r="G68" s="28"/>
       <c r="H68" s="28"/>
       <c r="I68" s="28"/>
-      <c r="J68" s="33"/>
-      <c r="K68" s="33"/>
-      <c r="L68" s="33"/>
-      <c r="M68" s="33"/>
-      <c r="N68" s="33"/>
-      <c r="O68" s="33"/>
-      <c r="P68" s="33"/>
-      <c r="Q68" s="33"/>
-      <c r="R68" s="33"/>
-      <c r="S68" s="33"/>
-      <c r="T68" s="33"/>
-      <c r="U68" s="33"/>
-      <c r="V68" s="33"/>
-      <c r="W68" s="33"/>
-      <c r="X68" s="33"/>
-      <c r="Y68" s="33"/>
-      <c r="Z68" s="33"/>
-      <c r="AA68" s="33"/>
-      <c r="AB68" s="33"/>
-      <c r="AC68" s="33"/>
-      <c r="AD68" s="33"/>
-      <c r="AE68" s="33"/>
-      <c r="AF68" s="33"/>
-      <c r="AG68" s="33"/>
-      <c r="AH68" s="33"/>
-      <c r="AI68" s="33"/>
-      <c r="AJ68" s="33"/>
-      <c r="AK68" s="33"/>
-      <c r="AL68" s="33"/>
-      <c r="AM68" s="33"/>
-      <c r="AN68" s="33"/>
-      <c r="AO68" s="33"/>
-      <c r="AP68" s="33"/>
-      <c r="AQ68" s="33"/>
-      <c r="AR68" s="33"/>
     </row>
-    <row r="69" spans="1:44" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:44" s="33" customFormat="1" ht="14">
       <c r="A69" s="29"/>
       <c r="B69" s="28"/>
       <c r="C69" s="28"/>
@@ -9363,7 +9304,7 @@
       <c r="H69" s="28"/>
       <c r="I69" s="28"/>
     </row>
-    <row r="70" spans="1:44" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:44" s="33" customFormat="1" ht="14">
       <c r="A70" s="29"/>
       <c r="B70" s="28"/>
       <c r="C70" s="28"/>
@@ -9374,7 +9315,7 @@
       <c r="H70" s="28"/>
       <c r="I70" s="28"/>
     </row>
-    <row r="71" spans="1:44" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:44" s="33" customFormat="1" ht="14">
       <c r="A71" s="29"/>
       <c r="B71" s="28"/>
       <c r="C71" s="28"/>
@@ -9385,407 +9326,407 @@
       <c r="H71" s="28"/>
       <c r="I71" s="28"/>
     </row>
-    <row r="72" spans="1:44" s="33" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="B72" s="40"/>
-      <c r="C72" s="40"/>
-      <c r="D72" s="40"/>
-      <c r="E72" s="40"/>
-      <c r="F72" s="40"/>
-      <c r="G72" s="40"/>
-      <c r="H72" s="40"/>
-      <c r="I72" s="40"/>
-      <c r="J72" s="40"/>
-      <c r="K72" s="40"/>
-      <c r="L72" s="40"/>
-      <c r="M72" s="40"/>
-      <c r="N72" s="40"/>
-      <c r="O72" s="40"/>
+    <row r="72" spans="1:44" s="33" customFormat="1" ht="94.5" customHeight="1">
+      <c r="A72" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B72" s="39"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="39"/>
+      <c r="F72" s="39"/>
+      <c r="G72" s="39"/>
+      <c r="H72" s="39"/>
+      <c r="I72" s="39"/>
+      <c r="J72" s="39"/>
+      <c r="K72" s="39"/>
+      <c r="L72" s="39"/>
+      <c r="M72" s="39"/>
+      <c r="N72" s="39"/>
+      <c r="O72" s="39"/>
       <c r="P72" s="34"/>
     </row>
-    <row r="73" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="40"/>
-      <c r="B73" s="40"/>
-      <c r="C73" s="40"/>
-      <c r="D73" s="40"/>
-      <c r="E73" s="40"/>
-      <c r="F73" s="40"/>
-      <c r="G73" s="40"/>
-      <c r="H73" s="40"/>
-      <c r="I73" s="40"/>
-      <c r="J73" s="40"/>
-      <c r="K73" s="40"/>
-      <c r="L73" s="40"/>
-      <c r="M73" s="40"/>
-      <c r="N73" s="40"/>
-      <c r="O73" s="40"/>
+    <row r="73" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A73" s="39"/>
+      <c r="B73" s="39"/>
+      <c r="C73" s="39"/>
+      <c r="D73" s="39"/>
+      <c r="E73" s="39"/>
+      <c r="F73" s="39"/>
+      <c r="G73" s="39"/>
+      <c r="H73" s="39"/>
+      <c r="I73" s="39"/>
+      <c r="J73" s="39"/>
+      <c r="K73" s="39"/>
+      <c r="L73" s="39"/>
+      <c r="M73" s="39"/>
+      <c r="N73" s="39"/>
+      <c r="O73" s="39"/>
       <c r="P73" s="34"/>
     </row>
-    <row r="74" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="40"/>
-      <c r="B74" s="40"/>
-      <c r="C74" s="40"/>
-      <c r="D74" s="40"/>
-      <c r="E74" s="40"/>
-      <c r="F74" s="40"/>
-      <c r="G74" s="40"/>
-      <c r="H74" s="40"/>
-      <c r="I74" s="40"/>
-      <c r="J74" s="40"/>
-      <c r="K74" s="40"/>
-      <c r="L74" s="40"/>
-      <c r="M74" s="40"/>
-      <c r="N74" s="40"/>
-      <c r="O74" s="40"/>
+    <row r="74" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A74" s="39"/>
+      <c r="B74" s="39"/>
+      <c r="C74" s="39"/>
+      <c r="D74" s="39"/>
+      <c r="E74" s="39"/>
+      <c r="F74" s="39"/>
+      <c r="G74" s="39"/>
+      <c r="H74" s="39"/>
+      <c r="I74" s="39"/>
+      <c r="J74" s="39"/>
+      <c r="K74" s="39"/>
+      <c r="L74" s="39"/>
+      <c r="M74" s="39"/>
+      <c r="N74" s="39"/>
+      <c r="O74" s="39"/>
       <c r="P74" s="34"/>
     </row>
-    <row r="75" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="40"/>
-      <c r="B75" s="40"/>
-      <c r="C75" s="40"/>
-      <c r="D75" s="40"/>
-      <c r="E75" s="40"/>
-      <c r="F75" s="40"/>
-      <c r="G75" s="40"/>
-      <c r="H75" s="40"/>
-      <c r="I75" s="40"/>
-      <c r="J75" s="40"/>
-      <c r="K75" s="40"/>
-      <c r="L75" s="40"/>
-      <c r="M75" s="40"/>
-      <c r="N75" s="40"/>
-      <c r="O75" s="40"/>
+    <row r="75" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A75" s="39"/>
+      <c r="B75" s="39"/>
+      <c r="C75" s="39"/>
+      <c r="D75" s="39"/>
+      <c r="E75" s="39"/>
+      <c r="F75" s="39"/>
+      <c r="G75" s="39"/>
+      <c r="H75" s="39"/>
+      <c r="I75" s="39"/>
+      <c r="J75" s="39"/>
+      <c r="K75" s="39"/>
+      <c r="L75" s="39"/>
+      <c r="M75" s="39"/>
+      <c r="N75" s="39"/>
+      <c r="O75" s="39"/>
       <c r="P75" s="34"/>
     </row>
-    <row r="76" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="40"/>
-      <c r="B76" s="40"/>
-      <c r="C76" s="40"/>
-      <c r="D76" s="40"/>
-      <c r="E76" s="40"/>
-      <c r="F76" s="40"/>
-      <c r="G76" s="40"/>
-      <c r="H76" s="40"/>
-      <c r="I76" s="40"/>
-      <c r="J76" s="40"/>
-      <c r="K76" s="40"/>
-      <c r="L76" s="40"/>
-      <c r="M76" s="40"/>
-      <c r="N76" s="40"/>
-      <c r="O76" s="40"/>
+    <row r="76" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A76" s="39"/>
+      <c r="B76" s="39"/>
+      <c r="C76" s="39"/>
+      <c r="D76" s="39"/>
+      <c r="E76" s="39"/>
+      <c r="F76" s="39"/>
+      <c r="G76" s="39"/>
+      <c r="H76" s="39"/>
+      <c r="I76" s="39"/>
+      <c r="J76" s="39"/>
+      <c r="K76" s="39"/>
+      <c r="L76" s="39"/>
+      <c r="M76" s="39"/>
+      <c r="N76" s="39"/>
+      <c r="O76" s="39"/>
       <c r="P76" s="34"/>
     </row>
-    <row r="77" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="40"/>
-      <c r="B77" s="40"/>
-      <c r="C77" s="40"/>
-      <c r="D77" s="40"/>
-      <c r="E77" s="40"/>
-      <c r="F77" s="40"/>
-      <c r="G77" s="40"/>
-      <c r="H77" s="40"/>
-      <c r="I77" s="40"/>
-      <c r="J77" s="40"/>
-      <c r="K77" s="40"/>
-      <c r="L77" s="40"/>
-      <c r="M77" s="40"/>
-      <c r="N77" s="40"/>
-      <c r="O77" s="40"/>
+    <row r="77" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A77" s="39"/>
+      <c r="B77" s="39"/>
+      <c r="C77" s="39"/>
+      <c r="D77" s="39"/>
+      <c r="E77" s="39"/>
+      <c r="F77" s="39"/>
+      <c r="G77" s="39"/>
+      <c r="H77" s="39"/>
+      <c r="I77" s="39"/>
+      <c r="J77" s="39"/>
+      <c r="K77" s="39"/>
+      <c r="L77" s="39"/>
+      <c r="M77" s="39"/>
+      <c r="N77" s="39"/>
+      <c r="O77" s="39"/>
       <c r="P77" s="34"/>
     </row>
-    <row r="78" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="40"/>
-      <c r="B78" s="40"/>
-      <c r="C78" s="40"/>
-      <c r="D78" s="40"/>
-      <c r="E78" s="40"/>
-      <c r="F78" s="40"/>
-      <c r="G78" s="40"/>
-      <c r="H78" s="40"/>
-      <c r="I78" s="40"/>
-      <c r="J78" s="40"/>
-      <c r="K78" s="40"/>
-      <c r="L78" s="40"/>
-      <c r="M78" s="40"/>
-      <c r="N78" s="40"/>
-      <c r="O78" s="40"/>
+    <row r="78" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A78" s="39"/>
+      <c r="B78" s="39"/>
+      <c r="C78" s="39"/>
+      <c r="D78" s="39"/>
+      <c r="E78" s="39"/>
+      <c r="F78" s="39"/>
+      <c r="G78" s="39"/>
+      <c r="H78" s="39"/>
+      <c r="I78" s="39"/>
+      <c r="J78" s="39"/>
+      <c r="K78" s="39"/>
+      <c r="L78" s="39"/>
+      <c r="M78" s="39"/>
+      <c r="N78" s="39"/>
+      <c r="O78" s="39"/>
       <c r="P78" s="34"/>
     </row>
-    <row r="79" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="40"/>
-      <c r="B79" s="40"/>
-      <c r="C79" s="40"/>
-      <c r="D79" s="40"/>
-      <c r="E79" s="40"/>
-      <c r="F79" s="40"/>
-      <c r="G79" s="40"/>
-      <c r="H79" s="40"/>
-      <c r="I79" s="40"/>
-      <c r="J79" s="40"/>
-      <c r="K79" s="40"/>
-      <c r="L79" s="40"/>
-      <c r="M79" s="40"/>
-      <c r="N79" s="40"/>
-      <c r="O79" s="40"/>
+    <row r="79" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A79" s="39"/>
+      <c r="B79" s="39"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="39"/>
+      <c r="E79" s="39"/>
+      <c r="F79" s="39"/>
+      <c r="G79" s="39"/>
+      <c r="H79" s="39"/>
+      <c r="I79" s="39"/>
+      <c r="J79" s="39"/>
+      <c r="K79" s="39"/>
+      <c r="L79" s="39"/>
+      <c r="M79" s="39"/>
+      <c r="N79" s="39"/>
+      <c r="O79" s="39"/>
       <c r="P79" s="34"/>
     </row>
-    <row r="80" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="40"/>
-      <c r="B80" s="40"/>
-      <c r="C80" s="40"/>
-      <c r="D80" s="40"/>
-      <c r="E80" s="40"/>
-      <c r="F80" s="40"/>
-      <c r="G80" s="40"/>
-      <c r="H80" s="40"/>
-      <c r="I80" s="40"/>
-      <c r="J80" s="40"/>
-      <c r="K80" s="40"/>
-      <c r="L80" s="40"/>
-      <c r="M80" s="40"/>
-      <c r="N80" s="40"/>
-      <c r="O80" s="40"/>
+    <row r="80" spans="1:44" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A80" s="39"/>
+      <c r="B80" s="39"/>
+      <c r="C80" s="39"/>
+      <c r="D80" s="39"/>
+      <c r="E80" s="39"/>
+      <c r="F80" s="39"/>
+      <c r="G80" s="39"/>
+      <c r="H80" s="39"/>
+      <c r="I80" s="39"/>
+      <c r="J80" s="39"/>
+      <c r="K80" s="39"/>
+      <c r="L80" s="39"/>
+      <c r="M80" s="39"/>
+      <c r="N80" s="39"/>
+      <c r="O80" s="39"/>
       <c r="P80" s="34"/>
     </row>
-    <row r="81" spans="1:16" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="40"/>
-      <c r="B81" s="40"/>
-      <c r="C81" s="40"/>
-      <c r="D81" s="40"/>
-      <c r="E81" s="40"/>
-      <c r="F81" s="40"/>
-      <c r="G81" s="40"/>
-      <c r="H81" s="40"/>
-      <c r="I81" s="40"/>
-      <c r="J81" s="40"/>
-      <c r="K81" s="40"/>
-      <c r="L81" s="40"/>
-      <c r="M81" s="40"/>
-      <c r="N81" s="40"/>
-      <c r="O81" s="40"/>
+    <row r="81" spans="1:16" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A81" s="39"/>
+      <c r="B81" s="39"/>
+      <c r="C81" s="39"/>
+      <c r="D81" s="39"/>
+      <c r="E81" s="39"/>
+      <c r="F81" s="39"/>
+      <c r="G81" s="39"/>
+      <c r="H81" s="39"/>
+      <c r="I81" s="39"/>
+      <c r="J81" s="39"/>
+      <c r="K81" s="39"/>
+      <c r="L81" s="39"/>
+      <c r="M81" s="39"/>
+      <c r="N81" s="39"/>
+      <c r="O81" s="39"/>
       <c r="P81" s="34"/>
     </row>
-    <row r="82" spans="1:16" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="40"/>
-      <c r="B82" s="40"/>
-      <c r="C82" s="40"/>
-      <c r="D82" s="40"/>
-      <c r="E82" s="40"/>
-      <c r="F82" s="40"/>
-      <c r="G82" s="40"/>
-      <c r="H82" s="40"/>
-      <c r="I82" s="40"/>
-      <c r="J82" s="40"/>
-      <c r="K82" s="40"/>
-      <c r="L82" s="40"/>
-      <c r="M82" s="40"/>
-      <c r="N82" s="40"/>
-      <c r="O82" s="40"/>
+    <row r="82" spans="1:16" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A82" s="39"/>
+      <c r="B82" s="39"/>
+      <c r="C82" s="39"/>
+      <c r="D82" s="39"/>
+      <c r="E82" s="39"/>
+      <c r="F82" s="39"/>
+      <c r="G82" s="39"/>
+      <c r="H82" s="39"/>
+      <c r="I82" s="39"/>
+      <c r="J82" s="39"/>
+      <c r="K82" s="39"/>
+      <c r="L82" s="39"/>
+      <c r="M82" s="39"/>
+      <c r="N82" s="39"/>
+      <c r="O82" s="39"/>
       <c r="P82" s="34"/>
     </row>
-    <row r="83" spans="1:16" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="40"/>
-      <c r="B83" s="40"/>
-      <c r="C83" s="40"/>
-      <c r="D83" s="40"/>
-      <c r="E83" s="40"/>
-      <c r="F83" s="40"/>
-      <c r="G83" s="40"/>
-      <c r="H83" s="40"/>
-      <c r="I83" s="40"/>
-      <c r="J83" s="40"/>
-      <c r="K83" s="40"/>
-      <c r="L83" s="40"/>
-      <c r="M83" s="40"/>
-      <c r="N83" s="40"/>
-      <c r="O83" s="40"/>
+    <row r="83" spans="1:16" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A83" s="39"/>
+      <c r="B83" s="39"/>
+      <c r="C83" s="39"/>
+      <c r="D83" s="39"/>
+      <c r="E83" s="39"/>
+      <c r="F83" s="39"/>
+      <c r="G83" s="39"/>
+      <c r="H83" s="39"/>
+      <c r="I83" s="39"/>
+      <c r="J83" s="39"/>
+      <c r="K83" s="39"/>
+      <c r="L83" s="39"/>
+      <c r="M83" s="39"/>
+      <c r="N83" s="39"/>
+      <c r="O83" s="39"/>
       <c r="P83" s="34"/>
     </row>
-    <row r="84" spans="1:16" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="40"/>
-      <c r="B84" s="40"/>
-      <c r="C84" s="40"/>
-      <c r="D84" s="40"/>
-      <c r="E84" s="40"/>
-      <c r="F84" s="40"/>
-      <c r="G84" s="40"/>
-      <c r="H84" s="40"/>
-      <c r="I84" s="40"/>
-      <c r="J84" s="40"/>
-      <c r="K84" s="40"/>
-      <c r="L84" s="40"/>
-      <c r="M84" s="40"/>
-      <c r="N84" s="40"/>
-      <c r="O84" s="40"/>
+    <row r="84" spans="1:16" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A84" s="39"/>
+      <c r="B84" s="39"/>
+      <c r="C84" s="39"/>
+      <c r="D84" s="39"/>
+      <c r="E84" s="39"/>
+      <c r="F84" s="39"/>
+      <c r="G84" s="39"/>
+      <c r="H84" s="39"/>
+      <c r="I84" s="39"/>
+      <c r="J84" s="39"/>
+      <c r="K84" s="39"/>
+      <c r="L84" s="39"/>
+      <c r="M84" s="39"/>
+      <c r="N84" s="39"/>
+      <c r="O84" s="39"/>
       <c r="P84" s="34"/>
     </row>
-    <row r="85" spans="1:16" s="33" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="40"/>
-      <c r="B85" s="40"/>
-      <c r="C85" s="40"/>
-      <c r="D85" s="40"/>
-      <c r="E85" s="40"/>
-      <c r="F85" s="40"/>
-      <c r="G85" s="40"/>
-      <c r="H85" s="40"/>
-      <c r="I85" s="40"/>
-      <c r="J85" s="40"/>
-      <c r="K85" s="40"/>
-      <c r="L85" s="40"/>
-      <c r="M85" s="40"/>
-      <c r="N85" s="40"/>
-      <c r="O85" s="40"/>
+    <row r="85" spans="1:16" s="33" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A85" s="39"/>
+      <c r="B85" s="39"/>
+      <c r="C85" s="39"/>
+      <c r="D85" s="39"/>
+      <c r="E85" s="39"/>
+      <c r="F85" s="39"/>
+      <c r="G85" s="39"/>
+      <c r="H85" s="39"/>
+      <c r="I85" s="39"/>
+      <c r="J85" s="39"/>
+      <c r="K85" s="39"/>
+      <c r="L85" s="39"/>
+      <c r="M85" s="39"/>
+      <c r="N85" s="39"/>
+      <c r="O85" s="39"/>
       <c r="P85" s="34"/>
     </row>
-    <row r="86" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="40"/>
-      <c r="B86" s="40"/>
-      <c r="C86" s="40"/>
-      <c r="D86" s="40"/>
-      <c r="E86" s="40"/>
-      <c r="F86" s="40"/>
-      <c r="G86" s="40"/>
-      <c r="H86" s="40"/>
-      <c r="I86" s="40"/>
-      <c r="J86" s="40"/>
-      <c r="K86" s="40"/>
-      <c r="L86" s="40"/>
-      <c r="M86" s="40"/>
-      <c r="N86" s="40"/>
-      <c r="O86" s="40"/>
+    <row r="86" spans="1:16" ht="12.75" customHeight="1">
+      <c r="A86" s="39"/>
+      <c r="B86" s="39"/>
+      <c r="C86" s="39"/>
+      <c r="D86" s="39"/>
+      <c r="E86" s="39"/>
+      <c r="F86" s="39"/>
+      <c r="G86" s="39"/>
+      <c r="H86" s="39"/>
+      <c r="I86" s="39"/>
+      <c r="J86" s="39"/>
+      <c r="K86" s="39"/>
+      <c r="L86" s="39"/>
+      <c r="M86" s="39"/>
+      <c r="N86" s="39"/>
+      <c r="O86" s="39"/>
     </row>
-    <row r="87" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="40"/>
-      <c r="B87" s="40"/>
-      <c r="C87" s="40"/>
-      <c r="D87" s="40"/>
-      <c r="E87" s="40"/>
-      <c r="F87" s="40"/>
-      <c r="G87" s="40"/>
-      <c r="H87" s="40"/>
-      <c r="I87" s="40"/>
-      <c r="J87" s="40"/>
-      <c r="K87" s="40"/>
-      <c r="L87" s="40"/>
-      <c r="M87" s="40"/>
-      <c r="N87" s="40"/>
-      <c r="O87" s="40"/>
+    <row r="87" spans="1:16" ht="12.75" customHeight="1">
+      <c r="A87" s="39"/>
+      <c r="B87" s="39"/>
+      <c r="C87" s="39"/>
+      <c r="D87" s="39"/>
+      <c r="E87" s="39"/>
+      <c r="F87" s="39"/>
+      <c r="G87" s="39"/>
+      <c r="H87" s="39"/>
+      <c r="I87" s="39"/>
+      <c r="J87" s="39"/>
+      <c r="K87" s="39"/>
+      <c r="L87" s="39"/>
+      <c r="M87" s="39"/>
+      <c r="N87" s="39"/>
+      <c r="O87" s="39"/>
     </row>
-    <row r="88" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="40"/>
-      <c r="B88" s="40"/>
-      <c r="C88" s="40"/>
-      <c r="D88" s="40"/>
-      <c r="E88" s="40"/>
-      <c r="F88" s="40"/>
-      <c r="G88" s="40"/>
-      <c r="H88" s="40"/>
-      <c r="I88" s="40"/>
-      <c r="J88" s="40"/>
-      <c r="K88" s="40"/>
-      <c r="L88" s="40"/>
-      <c r="M88" s="40"/>
-      <c r="N88" s="40"/>
-      <c r="O88" s="40"/>
+    <row r="88" spans="1:16" ht="12.75" customHeight="1">
+      <c r="A88" s="39"/>
+      <c r="B88" s="39"/>
+      <c r="C88" s="39"/>
+      <c r="D88" s="39"/>
+      <c r="E88" s="39"/>
+      <c r="F88" s="39"/>
+      <c r="G88" s="39"/>
+      <c r="H88" s="39"/>
+      <c r="I88" s="39"/>
+      <c r="J88" s="39"/>
+      <c r="K88" s="39"/>
+      <c r="L88" s="39"/>
+      <c r="M88" s="39"/>
+      <c r="N88" s="39"/>
+      <c r="O88" s="39"/>
     </row>
-    <row r="89" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="40"/>
-      <c r="B89" s="40"/>
-      <c r="C89" s="40"/>
-      <c r="D89" s="40"/>
-      <c r="E89" s="40"/>
-      <c r="F89" s="40"/>
-      <c r="G89" s="40"/>
-      <c r="H89" s="40"/>
-      <c r="I89" s="40"/>
-      <c r="J89" s="40"/>
-      <c r="K89" s="40"/>
-      <c r="L89" s="40"/>
-      <c r="M89" s="40"/>
-      <c r="N89" s="40"/>
-      <c r="O89" s="40"/>
+    <row r="89" spans="1:16" ht="12.75" customHeight="1">
+      <c r="A89" s="39"/>
+      <c r="B89" s="39"/>
+      <c r="C89" s="39"/>
+      <c r="D89" s="39"/>
+      <c r="E89" s="39"/>
+      <c r="F89" s="39"/>
+      <c r="G89" s="39"/>
+      <c r="H89" s="39"/>
+      <c r="I89" s="39"/>
+      <c r="J89" s="39"/>
+      <c r="K89" s="39"/>
+      <c r="L89" s="39"/>
+      <c r="M89" s="39"/>
+      <c r="N89" s="39"/>
+      <c r="O89" s="39"/>
     </row>
-    <row r="90" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="40"/>
-      <c r="B90" s="40"/>
-      <c r="C90" s="40"/>
-      <c r="D90" s="40"/>
-      <c r="E90" s="40"/>
-      <c r="F90" s="40"/>
-      <c r="G90" s="40"/>
-      <c r="H90" s="40"/>
-      <c r="I90" s="40"/>
-      <c r="J90" s="40"/>
-      <c r="K90" s="40"/>
-      <c r="L90" s="40"/>
-      <c r="M90" s="40"/>
-      <c r="N90" s="40"/>
-      <c r="O90" s="40"/>
+    <row r="90" spans="1:16" ht="12.75" customHeight="1">
+      <c r="A90" s="39"/>
+      <c r="B90" s="39"/>
+      <c r="C90" s="39"/>
+      <c r="D90" s="39"/>
+      <c r="E90" s="39"/>
+      <c r="F90" s="39"/>
+      <c r="G90" s="39"/>
+      <c r="H90" s="39"/>
+      <c r="I90" s="39"/>
+      <c r="J90" s="39"/>
+      <c r="K90" s="39"/>
+      <c r="L90" s="39"/>
+      <c r="M90" s="39"/>
+      <c r="N90" s="39"/>
+      <c r="O90" s="39"/>
     </row>
-    <row r="91" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="40"/>
-      <c r="B91" s="40"/>
-      <c r="C91" s="40"/>
-      <c r="D91" s="40"/>
-      <c r="E91" s="40"/>
-      <c r="F91" s="40"/>
-      <c r="G91" s="40"/>
-      <c r="H91" s="40"/>
-      <c r="I91" s="40"/>
-      <c r="J91" s="40"/>
-      <c r="K91" s="40"/>
-      <c r="L91" s="40"/>
-      <c r="M91" s="40"/>
-      <c r="N91" s="40"/>
-      <c r="O91" s="40"/>
+    <row r="91" spans="1:16" ht="12.75" customHeight="1">
+      <c r="A91" s="39"/>
+      <c r="B91" s="39"/>
+      <c r="C91" s="39"/>
+      <c r="D91" s="39"/>
+      <c r="E91" s="39"/>
+      <c r="F91" s="39"/>
+      <c r="G91" s="39"/>
+      <c r="H91" s="39"/>
+      <c r="I91" s="39"/>
+      <c r="J91" s="39"/>
+      <c r="K91" s="39"/>
+      <c r="L91" s="39"/>
+      <c r="M91" s="39"/>
+      <c r="N91" s="39"/>
+      <c r="O91" s="39"/>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A92" s="40"/>
-      <c r="B92" s="40"/>
-      <c r="C92" s="40"/>
-      <c r="D92" s="40"/>
-      <c r="E92" s="40"/>
-      <c r="F92" s="40"/>
-      <c r="G92" s="40"/>
-      <c r="H92" s="40"/>
-      <c r="I92" s="40"/>
-      <c r="J92" s="40"/>
-      <c r="K92" s="40"/>
-      <c r="L92" s="40"/>
-      <c r="M92" s="40"/>
-      <c r="N92" s="40"/>
-      <c r="O92" s="40"/>
+    <row r="92" spans="1:16">
+      <c r="A92" s="39"/>
+      <c r="B92" s="39"/>
+      <c r="C92" s="39"/>
+      <c r="D92" s="39"/>
+      <c r="E92" s="39"/>
+      <c r="F92" s="39"/>
+      <c r="G92" s="39"/>
+      <c r="H92" s="39"/>
+      <c r="I92" s="39"/>
+      <c r="J92" s="39"/>
+      <c r="K92" s="39"/>
+      <c r="L92" s="39"/>
+      <c r="M92" s="39"/>
+      <c r="N92" s="39"/>
+      <c r="O92" s="39"/>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A93" s="40"/>
-      <c r="B93" s="40"/>
-      <c r="C93" s="40"/>
-      <c r="D93" s="40"/>
-      <c r="E93" s="40"/>
-      <c r="F93" s="40"/>
-      <c r="G93" s="40"/>
-      <c r="H93" s="40"/>
-      <c r="I93" s="40"/>
-      <c r="J93" s="40"/>
-      <c r="K93" s="40"/>
-      <c r="L93" s="40"/>
-      <c r="M93" s="40"/>
-      <c r="N93" s="40"/>
-      <c r="O93" s="40"/>
+    <row r="93" spans="1:16">
+      <c r="A93" s="39"/>
+      <c r="B93" s="39"/>
+      <c r="C93" s="39"/>
+      <c r="D93" s="39"/>
+      <c r="E93" s="39"/>
+      <c r="F93" s="39"/>
+      <c r="G93" s="39"/>
+      <c r="H93" s="39"/>
+      <c r="I93" s="39"/>
+      <c r="J93" s="39"/>
+      <c r="K93" s="39"/>
+      <c r="L93" s="39"/>
+      <c r="M93" s="39"/>
+      <c r="N93" s="39"/>
+      <c r="O93" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A72:O93"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="B3:AK62">
-    <cfRule type="cellIs" dxfId="1" priority="32" operator="lessThan">
+  <conditionalFormatting sqref="B4:AR62">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL3:AR62">
+  <conditionalFormatting sqref="B3:AR3">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>